<commit_message>
fix: merge building_setup into buildings table for simplified onboarding
- Created migration to add structure_type, client_type, client_name, client_contact, client_email, and operational_notes columns to buildings table
- Removed separate Building Setup sheet from Excel template
- Merged building setup fields directly into Buildings sheet
- Updated import script to handle new unified structure
- Removed apportionments and compliance import sections (not in simplified template)
- Updated CSV upload guide to reflect changes
- Template now has only: Buildings, Units, Leaseholders, Leases

This eliminates confusion by ensuring the Excel template matches the actual database schema without requiring a separate building_setup table.

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/public/BlocIQ_Onboarding_Template_Simple.xlsx
+++ b/public/BlocIQ_Onboarding_Template_Simple.xlsx
@@ -5,18 +5,17 @@
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
     <sheet sheetId="1" name="Buildings" state="visible" r:id="rId4"/>
-    <sheet sheetId="2" name="Building Setup" state="visible" r:id="rId5"/>
-    <sheet sheetId="3" name="Units" state="visible" r:id="rId6"/>
-    <sheet sheetId="4" name="Leaseholders" state="visible" r:id="rId7"/>
-    <sheet sheetId="5" name="Leases" state="visible" r:id="rId8"/>
-    <sheet sheetId="6" name="Instructions" state="visible" r:id="rId9"/>
+    <sheet sheetId="2" name="Units" state="visible" r:id="rId5"/>
+    <sheet sheetId="3" name="Leaseholders" state="visible" r:id="rId6"/>
+    <sheet sheetId="4" name="Leases" state="visible" r:id="rId7"/>
+    <sheet sheetId="5" name="Instructions" state="visible" r:id="rId8"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="110">
   <si>
     <t>name</t>
   </si>
@@ -27,6 +26,24 @@
     <t>unit_count</t>
   </si>
   <si>
+    <t>structure_type</t>
+  </si>
+  <si>
+    <t>client_type</t>
+  </si>
+  <si>
+    <t>client_name</t>
+  </si>
+  <si>
+    <t>client_contact</t>
+  </si>
+  <si>
+    <t>client_email</t>
+  </si>
+  <si>
+    <t>operational_notes</t>
+  </si>
+  <si>
     <t>access_notes</t>
   </si>
   <si>
@@ -120,6 +137,24 @@
     <t>123 Main Street, London</t>
   </si>
   <si>
+    <t>RMC</t>
+  </si>
+  <si>
+    <t>Board of Directors</t>
+  </si>
+  <si>
+    <t>Pimlico Place Management Company Limited</t>
+  </si>
+  <si>
+    <t>Board Secretary</t>
+  </si>
+  <si>
+    <t>board@pimlicoplace.com</t>
+  </si>
+  <si>
+    <t>Regular board meetings quarterly</t>
+  </si>
+  <si>
     <t>Key code entry</t>
   </si>
   <si>
@@ -180,51 +215,15 @@
     <t>Delete this example row before importing</t>
   </si>
   <si>
+    <t>NOTE: structure_type must be: Freehold, RMC, Tripartite, RTM, or Leasehold</t>
+  </si>
+  <si>
+    <t>NOTE: client_type must be: Freeholder Company, Board of Directors, or Management Company</t>
+  </si>
+  <si>
     <t>building_name</t>
   </si>
   <si>
-    <t>structure_type</t>
-  </si>
-  <si>
-    <t>operational_notes</t>
-  </si>
-  <si>
-    <t>client_type</t>
-  </si>
-  <si>
-    <t>client_name</t>
-  </si>
-  <si>
-    <t>client_contact</t>
-  </si>
-  <si>
-    <t>client_email</t>
-  </si>
-  <si>
-    <t>RMC</t>
-  </si>
-  <si>
-    <t>Regular board meetings quarterly</t>
-  </si>
-  <si>
-    <t>Board of Directors</t>
-  </si>
-  <si>
-    <t>Pimlico Place Management Company Limited</t>
-  </si>
-  <si>
-    <t>Board Secretary</t>
-  </si>
-  <si>
-    <t>board@pimlicoplace.com</t>
-  </si>
-  <si>
-    <t>NOTE: structure_type must be: Freehold, RMC, or Tripartite</t>
-  </si>
-  <si>
-    <t>NOTE: client_type must be: Freeholder Company or Board of Directors</t>
-  </si>
-  <si>
     <t>unit_number</t>
   </si>
   <si>
@@ -309,27 +308,24 @@
     <t>Instructions</t>
   </si>
   <si>
-    <t>Fill in the Buildings sheet with your building information. Use exact database column names as headers.</t>
+    <t>Fill in the Buildings sheet with your building information including structure type and client details. Use exact database column names as headers.</t>
   </si>
   <si>
     <t>2</t>
   </si>
   <si>
-    <t>Fill in the Building Setup sheet (optional) with structure type and client information.</t>
+    <t>Fill in the Units sheet with unit information. Make sure building_name matches exactly from Buildings sheet.</t>
   </si>
   <si>
     <t>3</t>
   </si>
   <si>
-    <t>Fill in the Units sheet with unit information. Make sure building_name matches exactly from Buildings sheet.</t>
+    <t>Fill in the Leaseholders sheet. Make sure building_name and unit_number match exactly from previous sheets.</t>
   </si>
   <si>
     <t>4</t>
   </si>
   <si>
-    <t>Fill in the Leaseholders sheet. Make sure building_name and unit_number match exactly from previous sheets.</t>
-  </si>
-  <si>
     <t>Fill in the Leases sheet (optional) with lease documents. Match building_name and unit_number exactly.</t>
   </si>
   <si>
@@ -348,14 +344,14 @@
     <t>To upload: Open each sheet, save as CSV, then upload to Supabase Table Editor at https://supabase.com/dashboard/project/xqxaatvykmaaynqeoemy/editor</t>
   </si>
   <si>
-    <t>Order matters: 1) Buildings first, 2) Building Setup, 3) Units, 4) Leaseholders, 5) Leases</t>
+    <t>Order matters: 1) Buildings first, 2) Units, 3) Leaseholders, 4) Leases</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <color theme="1"/>
       <family val="2"/>
@@ -366,6 +362,10 @@
     <font>
       <b/>
       <color rgb="FFFFFFFF"/>
+    </font>
+    <font>
+      <i/>
+      <color rgb="FFFF6600"/>
     </font>
     <font>
       <i/>
@@ -421,7 +421,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -438,6 +438,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -777,38 +778,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF2"/>
+  <dimension ref="A1:AL3"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="30" customWidth="1"/>
     <col min="2" max="2" width="40" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="6" width="30" customWidth="1"/>
-    <col min="7" max="7" width="20" customWidth="1"/>
-    <col min="8" max="8" width="25" customWidth="1"/>
-    <col min="9" max="9" width="30" customWidth="1"/>
-    <col min="10" max="10" width="20" customWidth="1"/>
-    <col min="11" max="11" width="25" customWidth="1"/>
-    <col min="12" max="12" width="20" customWidth="1"/>
-    <col min="13" max="13" width="15" customWidth="1"/>
-    <col min="14" max="14" width="20" customWidth="1"/>
-    <col min="15" max="15" width="12" customWidth="1"/>
-    <col min="16" max="16" width="15" customWidth="1"/>
-    <col min="17" max="19" width="20" customWidth="1"/>
-    <col min="20" max="21" width="30" customWidth="1"/>
-    <col min="22" max="22" width="25" customWidth="1"/>
-    <col min="23" max="24" width="20" customWidth="1"/>
-    <col min="25" max="25" width="15" customWidth="1"/>
-    <col min="26" max="26" width="25" customWidth="1"/>
-    <col min="27" max="27" width="20" customWidth="1"/>
+    <col min="4" max="4" width="20" customWidth="1"/>
+    <col min="5" max="5" width="25" customWidth="1"/>
+    <col min="6" max="6" width="40" customWidth="1"/>
+    <col min="7" max="7" width="25" customWidth="1"/>
+    <col min="8" max="8" width="30" customWidth="1"/>
+    <col min="9" max="9" width="40" customWidth="1"/>
+    <col min="10" max="12" width="30" customWidth="1"/>
+    <col min="13" max="13" width="20" customWidth="1"/>
+    <col min="14" max="14" width="25" customWidth="1"/>
+    <col min="15" max="15" width="30" customWidth="1"/>
+    <col min="16" max="16" width="20" customWidth="1"/>
+    <col min="17" max="17" width="25" customWidth="1"/>
+    <col min="18" max="18" width="20" customWidth="1"/>
+    <col min="19" max="19" width="15" customWidth="1"/>
+    <col min="20" max="20" width="20" customWidth="1"/>
+    <col min="21" max="21" width="12" customWidth="1"/>
+    <col min="22" max="22" width="15" customWidth="1"/>
+    <col min="23" max="25" width="20" customWidth="1"/>
+    <col min="26" max="27" width="30" customWidth="1"/>
     <col min="28" max="28" width="25" customWidth="1"/>
-    <col min="29" max="29" width="40" customWidth="1"/>
-    <col min="30" max="30" width="30" customWidth="1"/>
+    <col min="29" max="30" width="20" customWidth="1"/>
     <col min="31" max="31" width="15" customWidth="1"/>
     <col min="32" max="32" width="25" customWidth="1"/>
+    <col min="33" max="33" width="20" customWidth="1"/>
+    <col min="34" max="34" width="25" customWidth="1"/>
+    <col min="35" max="35" width="40" customWidth="1"/>
+    <col min="36" max="36" width="30" customWidth="1"/>
+    <col min="37" max="37" width="15" customWidth="1"/>
+    <col min="38" max="38" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="25" customHeight="1" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" ht="25" customHeight="1" spans="1:38" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -905,79 +912,123 @@
       <c r="AF1" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AG1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C2">
         <v>24</v>
       </c>
       <c r="D2" t="s">
-        <v>34</v>
+        <v>40</v>
+      </c>
+      <c r="E2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" t="s">
+        <v>42</v>
       </c>
       <c r="G2" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="H2" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="I2" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="J2" t="s">
-        <v>38</v>
-      </c>
-      <c r="K2" t="s">
-        <v>39</v>
-      </c>
-      <c r="L2" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="M2" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="N2" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="O2" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="P2" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="Q2" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="R2" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="S2" t="s">
-        <v>47</v>
+        <v>53</v>
+      </c>
+      <c r="T2" t="s">
+        <v>54</v>
+      </c>
+      <c r="U2" t="s">
+        <v>55</v>
+      </c>
+      <c r="V2" t="s">
+        <v>56</v>
       </c>
       <c r="W2" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="X2" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="Y2" t="s">
-        <v>50</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>51</v>
-      </c>
-      <c r="AA2">
+        <v>59</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>63</v>
+      </c>
+      <c r="AG2">
         <v>350</v>
       </c>
-      <c r="AB2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>53</v>
+      <c r="AH2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D3" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -987,80 +1038,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
-  <cols>
-    <col min="1" max="1" width="30" customWidth="1"/>
-    <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="40" customWidth="1"/>
-    <col min="4" max="4" width="25" customWidth="1"/>
-    <col min="5" max="5" width="30" customWidth="1"/>
-    <col min="6" max="6" width="25" customWidth="1"/>
-    <col min="7" max="7" width="30" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="25" customHeight="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D2" t="s">
-        <v>63</v>
-      </c>
-      <c r="E2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F2" t="s">
-        <v>65</v>
-      </c>
-      <c r="G2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
@@ -1073,7 +1050,7 @@
   <sheetData>
     <row r="1" ht="25" customHeight="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>69</v>
@@ -1087,7 +1064,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B2" t="s">
         <v>72</v>
@@ -1101,7 +1078,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B3" t="s">
         <v>75</v>
@@ -1119,7 +1096,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
@@ -1133,7 +1110,7 @@
   <sheetData>
     <row r="1" ht="25" customHeight="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>69</v>
@@ -1150,7 +1127,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B2" t="s">
         <v>72</v>
@@ -1167,7 +1144,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B3" t="s">
         <v>75</v>
@@ -1188,7 +1165,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G3"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
@@ -1202,7 +1179,7 @@
   <sheetData>
     <row r="1" ht="25" customHeight="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>69</v>
@@ -1225,7 +1202,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B2" t="s">
         <v>72</v>
@@ -1247,7 +1224,7 @@
       </c>
     </row>
     <row r="3" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="6" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1257,20 +1234,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B10"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
     <col min="2" max="2" width="100" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="30" customHeight="1" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" ht="30" customHeight="1" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="7" t="s">
         <v>96</v>
       </c>
     </row>
@@ -1308,9 +1285,9 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>104</v>
       </c>
     </row>
@@ -1318,40 +1295,32 @@
       <c r="A7" t="s">
         <v>105</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>105</v>
+      <c r="B7" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B8" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B9" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B10" t="s">
         <v>109</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>105</v>
-      </c>
-      <c r="B11" t="s">
-        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>